<commit_message>
changed to webdriver manager
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harish.meda\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harish.meda\Documents\GitHub\RS_automation\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5400" windowWidth="14380" windowHeight="4190"/>
+    <workbookView xWindow="0" yWindow="6600" windowWidth="14380" windowHeight="4190"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="8">
   <si>
     <t>CityAndState</t>
   </si>
@@ -27,22 +27,22 @@
     <t>HomePageUrl</t>
   </si>
   <si>
-    <t>https://master.d1kf438yw3sssi.amplifyapp.com/</t>
-  </si>
-  <si>
-    <t>https://master.d1kf438yw3sssi.amplifyapp.com/or/morrow-county/boardman/foreclosures</t>
-  </si>
-  <si>
     <t>SRPPageURL</t>
   </si>
   <si>
     <t>Boardman,OR</t>
   </si>
   <si>
-    <t>Woodland Hills,CA</t>
-  </si>
-  <si>
-    <t>https://master.d1kf438yw3sssi.amplifyapp.com/ca/los-angeles-county/woodland-hills/foreclosures</t>
+    <t>https://www.realtystore.com/</t>
+  </si>
+  <si>
+    <t>https://www.realtystore.com/or/morrow-county/boardman/foreclosures</t>
+  </si>
+  <si>
+    <t>Los Angeles, CA</t>
+  </si>
+  <si>
+    <t>https://www.realtystore.com/ca/los-angeles-county/los-angeles/foreclosures</t>
   </si>
 </sst>
 </file>
@@ -88,10 +88,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -312,10 +311,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD25"/>
+      <selection activeCell="C3" sqref="C3:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -333,18 +332,18 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -352,9 +351,97 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -362,6 +449,11 @@
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1"/>
     <hyperlink ref="C2" r:id="rId2"/>
+    <hyperlink ref="B3" r:id="rId3"/>
+    <hyperlink ref="B2" r:id="rId4"/>
+    <hyperlink ref="B4" r:id="rId5"/>
+    <hyperlink ref="B5:B11" r:id="rId6" display="https://www.realtystore.com/"/>
+    <hyperlink ref="C4:C11" r:id="rId7" display="https://www.realtystore.com/ca/los-angeles-county/los-angeles/foreclosures"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>